<commit_message>
key api report excel write
</commit_message>
<xml_diff>
--- a/Datas/test_apidata.xlsx
+++ b/Datas/test_apidata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="82">
   <si>
     <t>conf_key</t>
   </si>
@@ -106,13 +106,67 @@
     <t>充2</t>
   </si>
   <si>
+    <t>save2dict</t>
+  </si>
+  <si>
+    <t>auser</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>${cc}mm</t>
+  </si>
+  <si>
+    <t>充3</t>
+  </si>
+  <si>
+    <t>saveparam</t>
+  </si>
+  <si>
+    <t>xcode</t>
+  </si>
+  <si>
+    <t>充4</t>
+  </si>
+  <si>
     <t>get_api</t>
   </si>
   <si>
     <t>get</t>
   </si>
   <si>
-    <t>saveparam</t>
+    <t>za={'a':'a1'}</t>
+  </si>
+  <si>
+    <t>充5</t>
+  </si>
+  <si>
+    <t>post_api</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>zss=${auser}</t>
+  </si>
+  <si>
+    <t>充6</t>
+  </si>
+  <si>
+    <t>get/${auser}</t>
+  </si>
+  <si>
+    <t>充7</t>
+  </si>
+  <si>
+    <t>savejson</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>headers,X-Amzn-Trace-Id</t>
   </si>
   <si>
     <t>email</t>
@@ -121,76 +175,22 @@
     <t>xx@162.com</t>
   </si>
   <si>
-    <t>充3</t>
-  </si>
-  <si>
     <t>token1xcode</t>
   </si>
   <si>
-    <t>充4</t>
-  </si>
-  <si>
     <t>a=xxxxxx</t>
   </si>
   <si>
-    <t>充5</t>
-  </si>
-  <si>
-    <t>savejson</t>
-  </si>
-  <si>
-    <t>next</t>
-  </si>
-  <si>
-    <t>headers,X-Amzn-Trace-Id</t>
-  </si>
-  <si>
-    <t>充6</t>
-  </si>
-  <si>
     <t>post_pi</t>
   </si>
   <si>
-    <t>post</t>
-  </si>
-  <si>
     <t>${next}</t>
   </si>
   <si>
-    <t>充7</t>
-  </si>
-  <si>
     <t>basic-auth</t>
   </si>
   <si>
     <t>${u_a}=${u_b}</t>
-  </si>
-  <si>
-    <t>save2dict</t>
-  </si>
-  <si>
-    <t>auser</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>${cc}mm</t>
-  </si>
-  <si>
-    <t>xcode</t>
-  </si>
-  <si>
-    <t>za={'a':'a1'}</t>
-  </si>
-  <si>
-    <t>post_api</t>
-  </si>
-  <si>
-    <t>zss=${auser}</t>
-  </si>
-  <si>
-    <t>get/${auser}</t>
   </si>
   <si>
     <t>assertInJson</t>
@@ -270,10 +270,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -301,14 +301,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -316,7 +308,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,21 +322,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -352,7 +329,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,6 +340,43 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -382,32 +396,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -421,8 +412,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,6 +443,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -455,13 +509,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,37 +617,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,122 +627,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -666,14 +666,10 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,30 +685,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -741,17 +713,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -767,6 +728,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -775,6 +751,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -783,10 +770,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
@@ -795,16 +782,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
@@ -816,116 +803,116 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -958,9 +945,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1375,7 +1359,7 @@
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1386,7 +1370,7 @@
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1397,7 +1381,7 @@
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1408,7 +1392,7 @@
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1417,12 +1401,12 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4"/>
     </row>
   </sheetData>
@@ -1441,7 +1425,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="$A4:$XFD7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1523,57 +1507,107 @@
       <c r="D3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="8"/>
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="4">
+        <v>20001</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="6"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="6"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="2"/>
       <c r="H7" s="6"/>
@@ -1581,12 +1615,24 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="6"/>
       <c r="I8" s="7"/>
@@ -1677,7 +1723,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A11" sqref="$A11:$XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1757,13 +1803,13 @@
         <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="6"/>
@@ -1778,13 +1824,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="F4" s="7">
         <v>20001</v>
@@ -1805,13 +1851,13 @@
         <v>36</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="6"/>
@@ -1826,16 +1872,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="6"/>
@@ -1850,16 +1896,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="6"/>
@@ -1877,13 +1923,13 @@
         <v>46</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="6"/>
@@ -1951,16 +1997,16 @@
         <v>28</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="7"/>
@@ -1974,13 +2020,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="F13" s="4">
         <v>20001</v>
@@ -2001,13 +2047,13 @@
         <v>36</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="6"/>
@@ -2022,16 +2068,16 @@
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="6"/>
@@ -2046,13 +2092,13 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="2"/>
@@ -2071,13 +2117,13 @@
         <v>46</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="6"/>
@@ -2092,7 +2138,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>58</v>
@@ -2140,7 +2186,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>64</v>
@@ -2162,7 +2208,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>66</v>
@@ -2292,10 +2338,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>77</v>
@@ -2316,7 +2362,7 @@
         <v>36</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>75</v>
@@ -2336,7 +2382,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>74</v>
@@ -2359,10 +2405,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>79</v>

</xml_diff>